<commit_message>
Added Spec Sheet + Preliminary Trade Study
</commit_message>
<xml_diff>
--- a/ElectricalReqMat.xlsx
+++ b/ElectricalReqMat.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AQaut\Documents\OffsetVentilator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F552DBC7-660C-445E-80A8-38F4FEA2ABD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180ACEF4-4A13-42E0-BD72-3F9E91E0FEC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sensors" sheetId="1" r:id="rId1"/>
+    <sheet name="Readouts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,19 +26,254 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>faef</t>
-  </si>
-  <si>
-    <t>tester</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+  <si>
+    <t>USER INTERACE</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>"Turn &amp; Click" / Potentiometer</t>
+  </si>
+  <si>
+    <t>PEC11R-4225F-S0024</t>
+  </si>
+  <si>
+    <t>Ease of Use</t>
+  </si>
+  <si>
+    <t>Scalability</t>
+  </si>
+  <si>
+    <t>Single control can be used for anything.</t>
+  </si>
+  <si>
+    <t>Requires menu navigation for all settings (SLOW)</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Elegant!</t>
+  </si>
+  <si>
+    <t>1 @ $1.53</t>
+  </si>
+  <si>
+    <t>Qty @ Cost</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>Intuitive up/down buttons for various parameters.</t>
+  </si>
+  <si>
+    <t>More features require more buttons.</t>
+  </si>
+  <si>
+    <t>Capacitive Touch Sensors</t>
+  </si>
+  <si>
+    <t>Lifetime</t>
+  </si>
+  <si>
+    <t>Rotation: &gt;30k cycles
+Button: &gt;20k cycles</t>
+  </si>
+  <si>
+    <t>Pick based on final form factor. Something like: MX1A-11NN</t>
+  </si>
+  <si>
+    <t>At least 5-6 @ ~$1.00 ea. (SMD are less)</t>
+  </si>
+  <si>
+    <t>&gt;50,000,000 cycles</t>
+  </si>
+  <si>
+    <t>Sensor pads can be constructed with conductive tape / foil</t>
+  </si>
+  <si>
+    <t>None (implemented in SW)</t>
+  </si>
+  <si>
+    <t>Intuitive up/down (capacitive) buttons for various parameters</t>
+  </si>
+  <si>
+    <t>More features require more (capacitive) buttons… but this is not expensive.</t>
+  </si>
+  <si>
+    <t>Ideally infinite</t>
+  </si>
+  <si>
+    <t>Need to carefully test to ensure sensitivity with/without PPE, etc.</t>
+  </si>
+  <si>
+    <t>PRESSURE SENSOR</t>
+  </si>
+  <si>
+    <t>FLOW RATE SENSOR</t>
+  </si>
+  <si>
+    <t>VISUAL READOUT</t>
+  </si>
+  <si>
+    <t>ALARM</t>
+  </si>
+  <si>
+    <t>BME280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ae-bst.resource.bosch.com/media/_tech/media/datasheets/BST-BME280-DS002.pdf </t>
+  </si>
+  <si>
+    <t>BMP180</t>
+  </si>
+  <si>
+    <t>MS5803-14BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sparkfun.com/products/12909 </t>
+  </si>
+  <si>
+    <t>MPXV7002</t>
+  </si>
+  <si>
+    <t>MPXV5010DP</t>
+  </si>
+  <si>
+    <t>ADP5100</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/differential-pressure-sensor-ics/7191184</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/gauge-pressure-sensor-ics/8368931</t>
+  </si>
+  <si>
+    <t>https://www.te.com/usa-en/product-CAT-BLPS0041.html</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0955598614001551</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Form Factor</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Range &amp; Accuracy</t>
+  </si>
+  <si>
+    <t>Digital Interface</t>
+  </si>
+  <si>
+    <t>2.5x2.5mm surface mount package w/ metal lid</t>
+  </si>
+  <si>
+    <t>I2C and SPI</t>
+  </si>
+  <si>
+    <t>Pressure Sensor Notes:
+UK requested: Normal pressure of 35 cmH2O, adjustable in increments of 5 cmH2O up to a potential maximum of 70 cm H2O (with PEEP in the range 5-20 cmH2O)
+1 cmH2O = 0.98 hPa
+Atmospheric pressure is 1,013 hPA</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Absolute</t>
+  </si>
+  <si>
+    <t>Includes humidity + temp. sensors</t>
+  </si>
+  <si>
+    <t>$6.55 sensor
+$20 SparkFun breakout</t>
+  </si>
+  <si>
+    <t>300 ~ 1100 hPa
++/- 1.0 hPa (0.12 hPa typ.)</t>
+  </si>
+  <si>
+    <t>Obsolete / Out of stock</t>
+  </si>
+  <si>
+    <t>$60 SparkFun breakout</t>
+  </si>
+  <si>
+    <t>Error = +/- 20 hPA at best</t>
+  </si>
+  <si>
+    <t>Range: +/- 20 hPA
++/- 2.5 hPa (1.0 hPa typ.)</t>
+  </si>
+  <si>
+    <t>$16.90 sensor</t>
+  </si>
+  <si>
+    <t>Differential</t>
+  </si>
+  <si>
+    <t>Analog Output</t>
+  </si>
+  <si>
+    <t>8-SOP, 8mm tall w/ 2 male ports</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?mpart=MPXV7002DP&amp;v=568</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>S-type Pitot tube using two pressure sensors?</t>
+  </si>
+  <si>
+    <t>Range: 0 ~ 100 hPA
+Error: 5 hPa</t>
+  </si>
+  <si>
+    <t>Temperature Compensated</t>
+  </si>
+  <si>
+    <t>$17.70 sensor</t>
+  </si>
+  <si>
+    <t>8-SOP, 10mm tall w/ 2 male ports</t>
+  </si>
+  <si>
+    <t>Range: +/- 1000 hPa
+Error: 13 hPa</t>
+  </si>
+  <si>
+    <t>MS4525 Series</t>
+  </si>
+  <si>
+    <t>MS45254525-DS5A001DP</t>
+  </si>
+  <si>
+    <t>Range: 0 ~ 68.9 hPa
+0.17 hPa</t>
+  </si>
+  <si>
+    <t>$39.31 sensor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +281,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,14 +332,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -348,45 +679,445 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D5:E10"/>
+  <dimension ref="C4:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+    <col min="8" max="9" width="21.77734375" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="3:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="3:11" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D16" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D21" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="3:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D21:J26"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K13" r:id="rId1" xr:uid="{50BD0665-7000-47E2-8DDA-3AA860FF01F1}"/>
+    <hyperlink ref="K15" r:id="rId2" xr:uid="{497BE04E-D5F8-4396-AFE1-F3346093BC92}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E137A05-B8E1-477C-BB75-D32BBC321682}">
+  <dimension ref="C3:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D10">
-        <v>4</v>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>